<commit_message>
Add tips to users.xls
</commit_message>
<xml_diff>
--- a/public/excels/user.xlsx
+++ b/public/excels/user.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26915"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kang/develop/rails/online_course/public/excels/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15940"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,6 +18,9 @@
   </sheets>
   <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -59,14 +67,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>年级</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>专业</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>specialty</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -86,10 +86,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>班级</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>grade2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -102,7 +98,34 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Q1</t>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>年级（年份）</t>
+    <rPh sb="3" eb="4">
+      <t>nian'fen</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>班级(班级号)</t>
+    <rPh sb="3" eb="4">
+      <t>ban'ji</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>hao'ma</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>专业（专业代码）</t>
+    <rPh sb="3" eb="4">
+      <t>zhuan'ye</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>dai'ma</t>
+    </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -227,6 +250,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="17">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -235,18 +259,22 @@
     <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -537,11 +565,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="28" style="1" customWidth="1"/>
     <col min="2" max="3" width="16.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="25.6640625" style="1" customWidth="1"/>
@@ -550,15 +580,15 @@
     <col min="8" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -573,18 +603,18 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
@@ -599,24 +629,24 @@
         <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>620203</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1">
         <v>20152354</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F3" s="2">
         <v>13381989831</v>
@@ -625,18 +655,13 @@
         <v>8</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -646,16 +671,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -665,15 +685,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>